<commit_message>
modify calc_elev_and_gradient to add soil properties
</commit_message>
<xml_diff>
--- a/ModelRuns/WeatheringParamStudy/model_parameter_and_output_summary_wxing_5x5x5.xlsx
+++ b/ModelRuns/WeatheringParamStudy/model_parameter_and_output_summary_wxing_5x5x5.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Data on Grain Hill runs with 5x5x5 parameter study of disturbance rate, weathering rate, and uplift interval</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>w</t>
+  </si>
+  <si>
+    <t>Runs for a 3x3 plot</t>
   </si>
 </sst>
 </file>
@@ -377,45 +380,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F134"/>
+  <dimension ref="A1:K134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="F127" sqref="F127"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -434,8 +437,11 @@
       <c r="F9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -457,7 +463,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
@@ -479,8 +485,17 @@
         <f>10^-2.5</f>
         <v>3.1622776601683764E-3</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I11">
+        <v>101</v>
+      </c>
+      <c r="J11">
+        <v>113</v>
+      </c>
+      <c r="K11">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>3</v>
       </c>
@@ -502,8 +517,20 @@
         <f>10^-2</f>
         <v>0.01</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H12" t="s">
+        <v>9</v>
+      </c>
+      <c r="I12">
+        <v>51</v>
+      </c>
+      <c r="J12">
+        <v>63</v>
+      </c>
+      <c r="K12">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>4</v>
       </c>
@@ -525,8 +552,17 @@
         <f>10^-1.5</f>
         <v>3.1622776601683784E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>13</v>
+      </c>
+      <c r="K13">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>5</v>
       </c>
@@ -548,8 +584,11 @@
         <f>0.1</f>
         <v>0.1</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>6</v>
       </c>
@@ -572,7 +611,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>7</v>
       </c>

</xml_diff>